<commit_message>
Revisiting core_bacteria and sequencing
</commit_message>
<xml_diff>
--- a/data/comparing_check_usual.xlsx
+++ b/data/comparing_check_usual.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE22"/>
+  <dimension ref="A1:BI34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2125,6 +2125,2412 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Dataset: core</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="E26" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="G26" s="1" t="n">
+        <v>177</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <v>270</v>
+      </c>
+      <c r="K26" s="1" t="n">
+        <v>304</v>
+      </c>
+      <c r="L26" s="1" t="n">
+        <v>371</v>
+      </c>
+      <c r="M26" s="1" t="n">
+        <v>449</v>
+      </c>
+      <c r="N26" s="1" t="n">
+        <v>462</v>
+      </c>
+      <c r="O26" s="1" t="n">
+        <v>550</v>
+      </c>
+      <c r="P26" s="1" t="n">
+        <v>589</v>
+      </c>
+      <c r="Q26" s="1" t="n">
+        <v>591</v>
+      </c>
+      <c r="R26" s="1" t="n">
+        <v>659</v>
+      </c>
+      <c r="S26" s="1" t="n">
+        <v>676</v>
+      </c>
+      <c r="T26" s="1" t="n">
+        <v>683</v>
+      </c>
+      <c r="U26" s="1" t="n">
+        <v>705</v>
+      </c>
+      <c r="V26" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="W26" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="X26" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="Y26" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="Z26" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA26" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB26" s="1" t="n">
+        <v>238</v>
+      </c>
+      <c r="AC26" s="1" t="n">
+        <v>245</v>
+      </c>
+      <c r="AD26" s="1" t="n">
+        <v>267</v>
+      </c>
+      <c r="AE26" s="1" t="n">
+        <v>271</v>
+      </c>
+      <c r="AF26" s="1" t="n">
+        <v>296</v>
+      </c>
+      <c r="AG26" s="1" t="n">
+        <v>344</v>
+      </c>
+      <c r="AH26" s="1" t="n">
+        <v>360</v>
+      </c>
+      <c r="AI26" s="1" t="n">
+        <v>484</v>
+      </c>
+      <c r="AJ26" s="1" t="n">
+        <v>575</v>
+      </c>
+      <c r="AK26" s="1" t="n">
+        <v>596</v>
+      </c>
+      <c r="AL26" s="1" t="n">
+        <v>634</v>
+      </c>
+      <c r="AM26" s="1" t="n">
+        <v>660</v>
+      </c>
+      <c r="AN26" s="1" t="n">
+        <v>664</v>
+      </c>
+      <c r="AO26" s="1" t="n">
+        <v>671</v>
+      </c>
+      <c r="AP26" s="1" t="n">
+        <v>674</v>
+      </c>
+      <c r="AQ26" s="1" t="n">
+        <v>715</v>
+      </c>
+      <c r="AR26" s="1" t="n">
+        <v>853</v>
+      </c>
+      <c r="AS26" s="1" t="n">
+        <v>863</v>
+      </c>
+      <c r="AT26" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="AU26" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="AV26" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="AW26" s="1" t="n">
+        <v>214</v>
+      </c>
+      <c r="AX26" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="AY26" s="1" t="n">
+        <v>229</v>
+      </c>
+      <c r="AZ26" s="1" t="n">
+        <v>354</v>
+      </c>
+      <c r="BA26" s="1" t="n">
+        <v>491</v>
+      </c>
+      <c r="BB26" s="1" t="n">
+        <v>572</v>
+      </c>
+      <c r="BC26" s="1" t="n">
+        <v>581</v>
+      </c>
+      <c r="BD26" s="1" t="n">
+        <v>587</v>
+      </c>
+      <c r="BE26" s="1" t="n">
+        <v>647</v>
+      </c>
+      <c r="BF26" s="1" t="n">
+        <v>687</v>
+      </c>
+      <c r="BG26" s="1" t="n">
+        <v>719</v>
+      </c>
+      <c r="BH26" s="1" t="n">
+        <v>731</v>
+      </c>
+      <c r="BI26" s="1" t="n">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Predominant Category</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>Cat 1</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AD27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AE27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AF27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AG27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AH27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AI27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AJ27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AK27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AL27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AM27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AN27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AO27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AP27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AQ27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AR27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AS27" t="inlineStr">
+        <is>
+          <t>Cat 2</t>
+        </is>
+      </c>
+      <c r="AT27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="AU27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="AV27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="AW27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="AX27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="AY27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="AZ27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BA27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BB27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BC27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BD27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BE27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BF27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BG27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BH27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+      <c r="BI27" t="inlineStr">
+        <is>
+          <t>Cat 3</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
+      <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" t="inlineStr"/>
+      <c r="AK28" t="inlineStr"/>
+      <c r="AL28" t="inlineStr"/>
+      <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr"/>
+      <c r="AO28" t="inlineStr"/>
+      <c r="AP28" t="inlineStr"/>
+      <c r="AQ28" t="inlineStr"/>
+      <c r="AR28" t="inlineStr"/>
+      <c r="AS28" t="inlineStr"/>
+      <c r="AT28" t="inlineStr"/>
+      <c r="AU28" t="inlineStr"/>
+      <c r="AV28" t="inlineStr"/>
+      <c r="AW28" t="inlineStr"/>
+      <c r="AX28" t="inlineStr"/>
+      <c r="AY28" t="inlineStr"/>
+      <c r="AZ28" t="inlineStr"/>
+      <c r="BA28" t="inlineStr"/>
+      <c r="BB28" t="inlineStr"/>
+      <c r="BC28" t="inlineStr"/>
+      <c r="BD28" t="inlineStr"/>
+      <c r="BE28" t="inlineStr"/>
+      <c r="BF28" t="inlineStr"/>
+      <c r="BG28" t="inlineStr"/>
+      <c r="BH28" t="inlineStr"/>
+      <c r="BI28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Frequency Cat 1</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>12/17 (70.6%)</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>13/17 (76.5%)</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>15/17 (88.2%)</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>15/17 (88.2%)</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>5/17 (29.4%)</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>15/17 (88.2%)</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>13/17 (76.5%)</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>12/17 (70.6%)</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>12/17 (70.6%)</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>12/17 (70.6%)</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>8/17 (47.1%)</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>14/17 (82.4%)</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>6/17 (35.3%)</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr">
+        <is>
+          <t>13/17 (76.5%)</t>
+        </is>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>17/17 (100.0%)</t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>0/17 (0.0%)</t>
+        </is>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>15/17 (88.2%)</t>
+        </is>
+      </c>
+      <c r="AD29" t="inlineStr">
+        <is>
+          <t>6/17 (35.3%)</t>
+        </is>
+      </c>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t>14/17 (82.4%)</t>
+        </is>
+      </c>
+      <c r="AF29" t="inlineStr">
+        <is>
+          <t>5/17 (29.4%)</t>
+        </is>
+      </c>
+      <c r="AG29" t="inlineStr">
+        <is>
+          <t>9/17 (52.9%)</t>
+        </is>
+      </c>
+      <c r="AH29" t="inlineStr">
+        <is>
+          <t>2/17 (11.8%)</t>
+        </is>
+      </c>
+      <c r="AI29" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="AJ29" t="inlineStr">
+        <is>
+          <t>15/17 (88.2%)</t>
+        </is>
+      </c>
+      <c r="AK29" t="inlineStr">
+        <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="AL29" t="inlineStr">
+        <is>
+          <t>7/17 (41.2%)</t>
+        </is>
+      </c>
+      <c r="AM29" t="inlineStr">
+        <is>
+          <t>8/17 (47.1%)</t>
+        </is>
+      </c>
+      <c r="AN29" t="inlineStr">
+        <is>
+          <t>11/17 (64.7%)</t>
+        </is>
+      </c>
+      <c r="AO29" t="inlineStr">
+        <is>
+          <t>14/17 (82.4%)</t>
+        </is>
+      </c>
+      <c r="AP29" t="inlineStr">
+        <is>
+          <t>13/17 (76.5%)</t>
+        </is>
+      </c>
+      <c r="AQ29" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="AR29" t="inlineStr">
+        <is>
+          <t>5/17 (29.4%)</t>
+        </is>
+      </c>
+      <c r="AS29" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="AT29" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="AU29" t="inlineStr">
+        <is>
+          <t>17/17 (100.0%)</t>
+        </is>
+      </c>
+      <c r="AV29" t="inlineStr">
+        <is>
+          <t>10/17 (58.8%)</t>
+        </is>
+      </c>
+      <c r="AW29" t="inlineStr">
+        <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="AX29" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="AY29" t="inlineStr">
+        <is>
+          <t>6/17 (35.3%)</t>
+        </is>
+      </c>
+      <c r="AZ29" t="inlineStr">
+        <is>
+          <t>4/17 (23.5%)</t>
+        </is>
+      </c>
+      <c r="BA29" t="inlineStr">
+        <is>
+          <t>16/17 (94.1%)</t>
+        </is>
+      </c>
+      <c r="BB29" t="inlineStr">
+        <is>
+          <t>13/17 (76.5%)</t>
+        </is>
+      </c>
+      <c r="BC29" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="BD29" t="inlineStr">
+        <is>
+          <t>16/17 (94.1%)</t>
+        </is>
+      </c>
+      <c r="BE29" t="inlineStr">
+        <is>
+          <t>12/17 (70.6%)</t>
+        </is>
+      </c>
+      <c r="BF29" t="inlineStr">
+        <is>
+          <t>14/17 (82.4%)</t>
+        </is>
+      </c>
+      <c r="BG29" t="inlineStr">
+        <is>
+          <t>1/17 (5.9%)</t>
+        </is>
+      </c>
+      <c r="BH29" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+      <c r="BI29" t="inlineStr">
+        <is>
+          <t>3/17 (17.6%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Abundance Mean Cat 1</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>0.7083</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2.2050</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.5737</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>3.5336</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>1.9595</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>1.6048</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>1.1143</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>4.4519</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>3.1918</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>2.1515</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>1.5768</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>1.4753</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>0.6568</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>3.3257</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>0.7111</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>3.0550</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>0.4935</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>0.9343</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>1.0229</t>
+        </is>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>0.6402</t>
+        </is>
+      </c>
+      <c r="V30" t="inlineStr">
+        <is>
+          <t>0.3955</t>
+        </is>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>0.1962</t>
+        </is>
+      </c>
+      <c r="X30" t="inlineStr">
+        <is>
+          <t>0.0001</t>
+        </is>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>1.5544</t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr">
+        <is>
+          <t>0.0004</t>
+        </is>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>0.0156</t>
+        </is>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>1.8058</t>
+        </is>
+      </c>
+      <c r="AD30" t="inlineStr">
+        <is>
+          <t>0.0183</t>
+        </is>
+      </c>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>1.0607</t>
+        </is>
+      </c>
+      <c r="AF30" t="inlineStr">
+        <is>
+          <t>0.0432</t>
+        </is>
+      </c>
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t>0.0466</t>
+        </is>
+      </c>
+      <c r="AH30" t="inlineStr">
+        <is>
+          <t>0.0014</t>
+        </is>
+      </c>
+      <c r="AI30" t="inlineStr">
+        <is>
+          <t>0.1862</t>
+        </is>
+      </c>
+      <c r="AJ30" t="inlineStr">
+        <is>
+          <t>0.7372</t>
+        </is>
+      </c>
+      <c r="AK30" t="inlineStr">
+        <is>
+          <t>0.0057</t>
+        </is>
+      </c>
+      <c r="AL30" t="inlineStr">
+        <is>
+          <t>0.0511</t>
+        </is>
+      </c>
+      <c r="AM30" t="inlineStr">
+        <is>
+          <t>0.4703</t>
+        </is>
+      </c>
+      <c r="AN30" t="inlineStr">
+        <is>
+          <t>1.6459</t>
+        </is>
+      </c>
+      <c r="AO30" t="inlineStr">
+        <is>
+          <t>2.4701</t>
+        </is>
+      </c>
+      <c r="AP30" t="inlineStr">
+        <is>
+          <t>0.4341</t>
+        </is>
+      </c>
+      <c r="AQ30" t="inlineStr">
+        <is>
+          <t>0.7020</t>
+        </is>
+      </c>
+      <c r="AR30" t="inlineStr">
+        <is>
+          <t>0.0106</t>
+        </is>
+      </c>
+      <c r="AS30" t="inlineStr">
+        <is>
+          <t>0.4485</t>
+        </is>
+      </c>
+      <c r="AT30" t="inlineStr">
+        <is>
+          <t>0.2679</t>
+        </is>
+      </c>
+      <c r="AU30" t="inlineStr">
+        <is>
+          <t>3.7249</t>
+        </is>
+      </c>
+      <c r="AV30" t="inlineStr">
+        <is>
+          <t>1.1960</t>
+        </is>
+      </c>
+      <c r="AW30" t="inlineStr">
+        <is>
+          <t>0.0743</t>
+        </is>
+      </c>
+      <c r="AX30" t="inlineStr">
+        <is>
+          <t>0.0002</t>
+        </is>
+      </c>
+      <c r="AY30" t="inlineStr">
+        <is>
+          <t>0.1092</t>
+        </is>
+      </c>
+      <c r="AZ30" t="inlineStr">
+        <is>
+          <t>0.0462</t>
+        </is>
+      </c>
+      <c r="BA30" t="inlineStr">
+        <is>
+          <t>1.1462</t>
+        </is>
+      </c>
+      <c r="BB30" t="inlineStr">
+        <is>
+          <t>5.9231</t>
+        </is>
+      </c>
+      <c r="BC30" t="inlineStr">
+        <is>
+          <t>0.1153</t>
+        </is>
+      </c>
+      <c r="BD30" t="inlineStr">
+        <is>
+          <t>1.8851</t>
+        </is>
+      </c>
+      <c r="BE30" t="inlineStr">
+        <is>
+          <t>3.5567</t>
+        </is>
+      </c>
+      <c r="BF30" t="inlineStr">
+        <is>
+          <t>0.6624</t>
+        </is>
+      </c>
+      <c r="BG30" t="inlineStr">
+        <is>
+          <t>0.0959</t>
+        </is>
+      </c>
+      <c r="BH30" t="inlineStr">
+        <is>
+          <t>0.5932</t>
+        </is>
+      </c>
+      <c r="BI30" t="inlineStr">
+        <is>
+          <t>0.0785</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Frequency Cat 2</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>10/32 (31.2%)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>4/32 (12.5%)</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>20/32 (62.5%)</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>28/32 (87.5%)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>21/32 (65.6%)</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>0/32 (0.0%)</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>14/32 (43.8%)</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>17/32 (53.1%)</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>12/32 (37.5%)</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>15/32 (46.9%)</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>9/32 (28.1%)</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>20/32 (62.5%)</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>9/32 (28.1%)</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>11/32 (34.4%)</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>12/32 (37.5%)</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>9/32 (28.1%)</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>16/32 (50.0%)</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>23/32 (71.9%)</t>
+        </is>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>11/32 (34.4%)</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr">
+        <is>
+          <t>17/32 (53.1%)</t>
+        </is>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>16/32 (50.0%)</t>
+        </is>
+      </c>
+      <c r="X31" t="inlineStr">
+        <is>
+          <t>1/32 (3.1%)</t>
+        </is>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>28/32 (87.5%)</t>
+        </is>
+      </c>
+      <c r="Z31" t="inlineStr">
+        <is>
+          <t>7/32 (21.9%)</t>
+        </is>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>12/32 (37.5%)</t>
+        </is>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>3/32 (9.4%)</t>
+        </is>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>24/32 (75.0%)</t>
+        </is>
+      </c>
+      <c r="AD31" t="inlineStr">
+        <is>
+          <t>9/32 (28.1%)</t>
+        </is>
+      </c>
+      <c r="AE31" t="inlineStr">
+        <is>
+          <t>20/32 (62.5%)</t>
+        </is>
+      </c>
+      <c r="AF31" t="inlineStr">
+        <is>
+          <t>11/32 (34.4%)</t>
+        </is>
+      </c>
+      <c r="AG31" t="inlineStr">
+        <is>
+          <t>20/32 (62.5%)</t>
+        </is>
+      </c>
+      <c r="AH31" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="AI31" t="inlineStr">
+        <is>
+          <t>11/32 (34.4%)</t>
+        </is>
+      </c>
+      <c r="AJ31" t="inlineStr">
+        <is>
+          <t>19/32 (59.4%)</t>
+        </is>
+      </c>
+      <c r="AK31" t="inlineStr">
+        <is>
+          <t>18/32 (56.2%)</t>
+        </is>
+      </c>
+      <c r="AL31" t="inlineStr">
+        <is>
+          <t>14/32 (43.8%)</t>
+        </is>
+      </c>
+      <c r="AM31" t="inlineStr">
+        <is>
+          <t>15/32 (46.9%)</t>
+        </is>
+      </c>
+      <c r="AN31" t="inlineStr">
+        <is>
+          <t>10/32 (31.2%)</t>
+        </is>
+      </c>
+      <c r="AO31" t="inlineStr">
+        <is>
+          <t>24/32 (75.0%)</t>
+        </is>
+      </c>
+      <c r="AP31" t="inlineStr">
+        <is>
+          <t>29/32 (90.6%)</t>
+        </is>
+      </c>
+      <c r="AQ31" t="inlineStr">
+        <is>
+          <t>11/32 (34.4%)</t>
+        </is>
+      </c>
+      <c r="AR31" t="inlineStr">
+        <is>
+          <t>13/32 (40.6%)</t>
+        </is>
+      </c>
+      <c r="AS31" t="inlineStr">
+        <is>
+          <t>19/32 (59.4%)</t>
+        </is>
+      </c>
+      <c r="AT31" t="inlineStr">
+        <is>
+          <t>4/32 (12.5%)</t>
+        </is>
+      </c>
+      <c r="AU31" t="inlineStr">
+        <is>
+          <t>26/32 (81.2%)</t>
+        </is>
+      </c>
+      <c r="AV31" t="inlineStr">
+        <is>
+          <t>17/32 (53.1%)</t>
+        </is>
+      </c>
+      <c r="AW31" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="AX31" t="inlineStr">
+        <is>
+          <t>1/32 (3.1%)</t>
+        </is>
+      </c>
+      <c r="AY31" t="inlineStr">
+        <is>
+          <t>12/32 (37.5%)</t>
+        </is>
+      </c>
+      <c r="AZ31" t="inlineStr">
+        <is>
+          <t>11/32 (34.4%)</t>
+        </is>
+      </c>
+      <c r="BA31" t="inlineStr">
+        <is>
+          <t>24/32 (75.0%)</t>
+        </is>
+      </c>
+      <c r="BB31" t="inlineStr">
+        <is>
+          <t>25/32 (78.1%)</t>
+        </is>
+      </c>
+      <c r="BC31" t="inlineStr">
+        <is>
+          <t>8/32 (25.0%)</t>
+        </is>
+      </c>
+      <c r="BD31" t="inlineStr">
+        <is>
+          <t>24/32 (75.0%)</t>
+        </is>
+      </c>
+      <c r="BE31" t="inlineStr">
+        <is>
+          <t>22/32 (68.8%)</t>
+        </is>
+      </c>
+      <c r="BF31" t="inlineStr">
+        <is>
+          <t>22/32 (68.8%)</t>
+        </is>
+      </c>
+      <c r="BG31" t="inlineStr">
+        <is>
+          <t>2/32 (6.2%)</t>
+        </is>
+      </c>
+      <c r="BH31" t="inlineStr">
+        <is>
+          <t>5/32 (15.6%)</t>
+        </is>
+      </c>
+      <c r="BI31" t="inlineStr">
+        <is>
+          <t>5/32 (15.6%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Abundance Mean Cat 2</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>0.3571</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>0.0043</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.4567</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>3.5277</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>1.3973</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>0.0271</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>0.8165</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>3.5785</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2.0406</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>0.8019</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>0.4458</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>0.2306</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>1.1314</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>1.4157</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>0.6543</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>0.4306</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>1.4856</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>0.3583</t>
+        </is>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>0.2283</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr">
+        <is>
+          <t>0.7538</t>
+        </is>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>1.4571</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr">
+        <is>
+          <t>1.5478</t>
+        </is>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>4.1919</t>
+        </is>
+      </c>
+      <c r="Z32" t="inlineStr">
+        <is>
+          <t>0.7206</t>
+        </is>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>0.8584</t>
+        </is>
+      </c>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>3.0723</t>
+        </is>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>3.5193</t>
+        </is>
+      </c>
+      <c r="AD32" t="inlineStr">
+        <is>
+          <t>0.9896</t>
+        </is>
+      </c>
+      <c r="AE32" t="inlineStr">
+        <is>
+          <t>3.0883</t>
+        </is>
+      </c>
+      <c r="AF32" t="inlineStr">
+        <is>
+          <t>1.6703</t>
+        </is>
+      </c>
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t>1.1083</t>
+        </is>
+      </c>
+      <c r="AH32" t="inlineStr">
+        <is>
+          <t>0.6756</t>
+        </is>
+      </c>
+      <c r="AI32" t="inlineStr">
+        <is>
+          <t>0.8460</t>
+        </is>
+      </c>
+      <c r="AJ32" t="inlineStr">
+        <is>
+          <t>3.3039</t>
+        </is>
+      </c>
+      <c r="AK32" t="inlineStr">
+        <is>
+          <t>0.9009</t>
+        </is>
+      </c>
+      <c r="AL32" t="inlineStr">
+        <is>
+          <t>0.9505</t>
+        </is>
+      </c>
+      <c r="AM32" t="inlineStr">
+        <is>
+          <t>0.6964</t>
+        </is>
+      </c>
+      <c r="AN32" t="inlineStr">
+        <is>
+          <t>4.0709</t>
+        </is>
+      </c>
+      <c r="AO32" t="inlineStr">
+        <is>
+          <t>2.8868</t>
+        </is>
+      </c>
+      <c r="AP32" t="inlineStr">
+        <is>
+          <t>1.8646</t>
+        </is>
+      </c>
+      <c r="AQ32" t="inlineStr">
+        <is>
+          <t>1.7617</t>
+        </is>
+      </c>
+      <c r="AR32" t="inlineStr">
+        <is>
+          <t>1.8953</t>
+        </is>
+      </c>
+      <c r="AS32" t="inlineStr">
+        <is>
+          <t>0.5028</t>
+        </is>
+      </c>
+      <c r="AT32" t="inlineStr">
+        <is>
+          <t>0.3296</t>
+        </is>
+      </c>
+      <c r="AU32" t="inlineStr">
+        <is>
+          <t>5.3619</t>
+        </is>
+      </c>
+      <c r="AV32" t="inlineStr">
+        <is>
+          <t>1.4407</t>
+        </is>
+      </c>
+      <c r="AW32" t="inlineStr">
+        <is>
+          <t>0.2834</t>
+        </is>
+      </c>
+      <c r="AX32" t="inlineStr">
+        <is>
+          <t>0.0001</t>
+        </is>
+      </c>
+      <c r="AY32" t="inlineStr">
+        <is>
+          <t>0.1405</t>
+        </is>
+      </c>
+      <c r="AZ32" t="inlineStr">
+        <is>
+          <t>1.6274</t>
+        </is>
+      </c>
+      <c r="BA32" t="inlineStr">
+        <is>
+          <t>1.5058</t>
+        </is>
+      </c>
+      <c r="BB32" t="inlineStr">
+        <is>
+          <t>3.9075</t>
+        </is>
+      </c>
+      <c r="BC32" t="inlineStr">
+        <is>
+          <t>0.8370</t>
+        </is>
+      </c>
+      <c r="BD32" t="inlineStr">
+        <is>
+          <t>5.6003</t>
+        </is>
+      </c>
+      <c r="BE32" t="inlineStr">
+        <is>
+          <t>0.5693</t>
+        </is>
+      </c>
+      <c r="BF32" t="inlineStr">
+        <is>
+          <t>0.5722</t>
+        </is>
+      </c>
+      <c r="BG32" t="inlineStr">
+        <is>
+          <t>0.1567</t>
+        </is>
+      </c>
+      <c r="BH32" t="inlineStr">
+        <is>
+          <t>0.3131</t>
+        </is>
+      </c>
+      <c r="BI32" t="inlineStr">
+        <is>
+          <t>0.3053</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Frequency Cat 3</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>14/21 (66.7%)</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>14/21 (66.7%)</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>14/21 (66.7%)</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>13/21 (61.9%)</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>13/21 (61.9%)</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>5/21 (23.8%)</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>15/21 (71.4%)</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>4/21 (19.0%)</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>14/21 (66.7%)</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>6/21 (28.6%)</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>7/21 (33.3%)</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>3/21 (14.3%)</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>10/21 (47.6%)</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>16/21 (76.2%)</t>
+        </is>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>20/21 (95.2%)</t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="AA33" t="inlineStr">
+        <is>
+          <t>3/21 (14.3%)</t>
+        </is>
+      </c>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t>0/21 (0.0%)</t>
+        </is>
+      </c>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>15/21 (71.4%)</t>
+        </is>
+      </c>
+      <c r="AD33" t="inlineStr">
+        <is>
+          <t>8/21 (38.1%)</t>
+        </is>
+      </c>
+      <c r="AE33" t="inlineStr">
+        <is>
+          <t>14/21 (66.7%)</t>
+        </is>
+      </c>
+      <c r="AF33" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="AG33" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="AH33" t="inlineStr">
+        <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="AI33" t="inlineStr">
+        <is>
+          <t>12/21 (57.1%)</t>
+        </is>
+      </c>
+      <c r="AJ33" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="AK33" t="inlineStr">
+        <is>
+          <t>8/21 (38.1%)</t>
+        </is>
+      </c>
+      <c r="AL33" t="inlineStr">
+        <is>
+          <t>3/21 (14.3%)</t>
+        </is>
+      </c>
+      <c r="AM33" t="inlineStr">
+        <is>
+          <t>6/21 (28.6%)</t>
+        </is>
+      </c>
+      <c r="AN33" t="inlineStr">
+        <is>
+          <t>4/21 (19.0%)</t>
+        </is>
+      </c>
+      <c r="AO33" t="inlineStr">
+        <is>
+          <t>16/21 (76.2%)</t>
+        </is>
+      </c>
+      <c r="AP33" t="inlineStr">
+        <is>
+          <t>19/21 (90.5%)</t>
+        </is>
+      </c>
+      <c r="AQ33" t="inlineStr">
+        <is>
+          <t>3/21 (14.3%)</t>
+        </is>
+      </c>
+      <c r="AR33" t="inlineStr">
+        <is>
+          <t>2/21 (9.5%)</t>
+        </is>
+      </c>
+      <c r="AS33" t="inlineStr">
+        <is>
+          <t>10/21 (47.6%)</t>
+        </is>
+      </c>
+      <c r="AT33" t="inlineStr">
+        <is>
+          <t>4/21 (19.0%)</t>
+        </is>
+      </c>
+      <c r="AU33" t="inlineStr">
+        <is>
+          <t>18/21 (85.7%)</t>
+        </is>
+      </c>
+      <c r="AV33" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="AW33" t="inlineStr">
+        <is>
+          <t>11/21 (52.4%)</t>
+        </is>
+      </c>
+      <c r="AX33" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="AY33" t="inlineStr">
+        <is>
+          <t>13/21 (61.9%)</t>
+        </is>
+      </c>
+      <c r="AZ33" t="inlineStr">
+        <is>
+          <t>13/21 (61.9%)</t>
+        </is>
+      </c>
+      <c r="BA33" t="inlineStr">
+        <is>
+          <t>20/21 (95.2%)</t>
+        </is>
+      </c>
+      <c r="BB33" t="inlineStr">
+        <is>
+          <t>19/21 (90.5%)</t>
+        </is>
+      </c>
+      <c r="BC33" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="BD33" t="inlineStr">
+        <is>
+          <t>18/21 (85.7%)</t>
+        </is>
+      </c>
+      <c r="BE33" t="inlineStr">
+        <is>
+          <t>16/21 (76.2%)</t>
+        </is>
+      </c>
+      <c r="BF33" t="inlineStr">
+        <is>
+          <t>14/21 (66.7%)</t>
+        </is>
+      </c>
+      <c r="BG33" t="inlineStr">
+        <is>
+          <t>1/21 (4.8%)</t>
+        </is>
+      </c>
+      <c r="BH33" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+      <c r="BI33" t="inlineStr">
+        <is>
+          <t>9/21 (42.9%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Abundance Mean Cat 3</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>0.3083</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0.5458</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>1.9188</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>0.6369</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>0.2031</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2.0780</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>1.5181</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>0.0963</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>0.1631</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>1.6504</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>0.3825</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>0.7315</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>0.1486</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>0.4269</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>0.1449</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>0.0828</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>0.3519</t>
+        </is>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>0.3982</t>
+        </is>
+      </c>
+      <c r="V34" t="inlineStr">
+        <is>
+          <t>0.3523</t>
+        </is>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>0.6954</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr">
+        <is>
+          <t>0.5614</t>
+        </is>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>1.4533</t>
+        </is>
+      </c>
+      <c r="Z34" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>0.0026</t>
+        </is>
+      </c>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>0.0000</t>
+        </is>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>2.1036</t>
+        </is>
+      </c>
+      <c r="AD34" t="inlineStr">
+        <is>
+          <t>0.0679</t>
+        </is>
+      </c>
+      <c r="AE34" t="inlineStr">
+        <is>
+          <t>1.3219</t>
+        </is>
+      </c>
+      <c r="AF34" t="inlineStr">
+        <is>
+          <t>0.1482</t>
+        </is>
+      </c>
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t>0.7162</t>
+        </is>
+      </c>
+      <c r="AH34" t="inlineStr">
+        <is>
+          <t>0.0004</t>
+        </is>
+      </c>
+      <c r="AI34" t="inlineStr">
+        <is>
+          <t>0.3615</t>
+        </is>
+      </c>
+      <c r="AJ34" t="inlineStr">
+        <is>
+          <t>2.7716</t>
+        </is>
+      </c>
+      <c r="AK34" t="inlineStr">
+        <is>
+          <t>0.0446</t>
+        </is>
+      </c>
+      <c r="AL34" t="inlineStr">
+        <is>
+          <t>0.1363</t>
+        </is>
+      </c>
+      <c r="AM34" t="inlineStr">
+        <is>
+          <t>0.2138</t>
+        </is>
+      </c>
+      <c r="AN34" t="inlineStr">
+        <is>
+          <t>0.5525</t>
+        </is>
+      </c>
+      <c r="AO34" t="inlineStr">
+        <is>
+          <t>1.5303</t>
+        </is>
+      </c>
+      <c r="AP34" t="inlineStr">
+        <is>
+          <t>0.3291</t>
+        </is>
+      </c>
+      <c r="AQ34" t="inlineStr">
+        <is>
+          <t>1.2484</t>
+        </is>
+      </c>
+      <c r="AR34" t="inlineStr">
+        <is>
+          <t>0.0008</t>
+        </is>
+      </c>
+      <c r="AS34" t="inlineStr">
+        <is>
+          <t>0.2533</t>
+        </is>
+      </c>
+      <c r="AT34" t="inlineStr">
+        <is>
+          <t>2.0973</t>
+        </is>
+      </c>
+      <c r="AU34" t="inlineStr">
+        <is>
+          <t>6.9495</t>
+        </is>
+      </c>
+      <c r="AV34" t="inlineStr">
+        <is>
+          <t>2.9782</t>
+        </is>
+      </c>
+      <c r="AW34" t="inlineStr">
+        <is>
+          <t>1.5101</t>
+        </is>
+      </c>
+      <c r="AX34" t="inlineStr">
+        <is>
+          <t>3.6990</t>
+        </is>
+      </c>
+      <c r="AY34" t="inlineStr">
+        <is>
+          <t>1.1856</t>
+        </is>
+      </c>
+      <c r="AZ34" t="inlineStr">
+        <is>
+          <t>2.7596</t>
+        </is>
+      </c>
+      <c r="BA34" t="inlineStr">
+        <is>
+          <t>4.9482</t>
+        </is>
+      </c>
+      <c r="BB34" t="inlineStr">
+        <is>
+          <t>6.4164</t>
+        </is>
+      </c>
+      <c r="BC34" t="inlineStr">
+        <is>
+          <t>0.8108</t>
+        </is>
+      </c>
+      <c r="BD34" t="inlineStr">
+        <is>
+          <t>5.3260</t>
+        </is>
+      </c>
+      <c r="BE34" t="inlineStr">
+        <is>
+          <t>3.9644</t>
+        </is>
+      </c>
+      <c r="BF34" t="inlineStr">
+        <is>
+          <t>1.4245</t>
+        </is>
+      </c>
+      <c r="BG34" t="inlineStr">
+        <is>
+          <t>1.3681</t>
+        </is>
+      </c>
+      <c r="BH34" t="inlineStr">
+        <is>
+          <t>2.3014</t>
+        </is>
+      </c>
+      <c r="BI34" t="inlineStr">
+        <is>
+          <t>1.0848</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>